<commit_message>
fixed design rule violations and added input diode
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D5C13C-579D-2746-A9F1-A041176F7248}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9875CD7E-6644-8544-AF72-E634B28D5314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10220" yWindow="29300" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -144,9 +144,6 @@
     <t>u</t>
   </si>
   <si>
-    <t>CN1, CN2, CN3</t>
-  </si>
-  <si>
     <t>Mega-Fit Right-Angle Header, Single Row, 5.70mm Pitch, 2 Circuits</t>
   </si>
   <si>
@@ -159,18 +156,9 @@
     <t>CN5</t>
   </si>
   <si>
-    <t>Mega-Fit Right-Angle Header, 8 Circuits, Tin (Sn) Plating</t>
-  </si>
-  <si>
     <t>1x2POS</t>
   </si>
   <si>
-    <t>2x4POS</t>
-  </si>
-  <si>
-    <t>CN6,CN7,CN8,CN9</t>
-  </si>
-  <si>
     <t>CONN HEADER R/A 2POS 2.54MM</t>
   </si>
   <si>
@@ -180,9 +168,6 @@
     <t>CUI Devices</t>
   </si>
   <si>
-    <t>CONN HEADER VERT 2POS 2.54MM</t>
-  </si>
-  <si>
     <t>Wurth Elektronik</t>
   </si>
   <si>
@@ -313,6 +298,39 @@
   </si>
   <si>
     <t>1x18POS</t>
+  </si>
+  <si>
+    <t>CN2,CN3,CN15</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 3POS 2.54MM</t>
+  </si>
+  <si>
+    <t>1x3POS</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 10POS 5.7MM</t>
+  </si>
+  <si>
+    <t>2x5POS</t>
+  </si>
+  <si>
+    <t>CN6,CN7,CN8,CN9,CN13,CN14</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>S1A-13-F</t>
+  </si>
+  <si>
+    <t>DIODE GEN PURP 50V 1A SMA</t>
+  </si>
+  <si>
+    <t>DO-214AC</t>
   </si>
 </sst>
 </file>
@@ -502,6 +520,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -513,9 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -872,13 +890,13 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9" style="3"/>
     <col min="4" max="4" width="24.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.83203125" style="3" customWidth="1"/>
@@ -890,25 +908,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="D2" s="26" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="D2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -944,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C7" s="7">
         <v>3</v>
@@ -956,13 +974,13 @@
         <v>2002411202</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>17</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>18</v>
       </c>
       <c r="I7" s="10"/>
     </row>
@@ -971,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
@@ -980,16 +998,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="8">
-        <v>705410036</v>
+        <v>1719710003</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="10"/>
     </row>
@@ -998,7 +1016,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="11">
         <v>1</v>
@@ -1007,16 +1025,16 @@
         <v>12</v>
       </c>
       <c r="E9" s="12">
-        <v>768250008</v>
+        <v>768250010</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" s="14"/>
     </row>
@@ -1025,10 +1043,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C10" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>12</v>
@@ -1037,13 +1055,13 @@
         <v>705530001</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" s="10"/>
     </row>
@@ -1052,25 +1070,25 @@
         <v>5</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" s="10"/>
     </row>
@@ -1079,25 +1097,25 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12" s="10"/>
     </row>
@@ -1106,23 +1124,23 @@
         <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E13" s="8">
         <v>3568</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="10"/>
     </row>
@@ -1131,19 +1149,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C14" s="7">
         <v>7</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>11</v>
@@ -1158,19 +1176,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>11</v>
@@ -1185,25 +1203,25 @@
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" s="10"/>
     </row>
@@ -1212,22 +1230,22 @@
         <v>11</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C17" s="11">
         <v>2</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>10</v>
@@ -1239,22 +1257,22 @@
         <v>12</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>10</v>
@@ -1266,22 +1284,22 @@
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="G19" s="15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>10</v>
@@ -1293,25 +1311,25 @@
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="10"/>
     </row>
@@ -1320,51 +1338,67 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C21" s="7">
         <v>2</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="10"/>
+      <c r="A22" s="7">
+        <v>16</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="I22" s="10"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="17"/>
@@ -1378,17 +1412,17 @@
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="37" spans="8:8">
       <c r="H37" s="3" t="s">

</xml_diff>

<commit_message>
laid out all components and got most footprints imported
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9875CD7E-6644-8544-AF72-E634B28D5314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1191C312-0608-2D44-889E-AD02AC08724D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="29300" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="10220" yWindow="29300" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
     <t>DIODE GEN PURP 50V 1A SMA</t>
   </si>
   <si>
-    <t>DO-214AC</t>
+    <t>SMA</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,7 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
finished first draft of PCB
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1191C312-0608-2D44-889E-AD02AC08724D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D3DC74-58AD-1E47-9236-83E176C978E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="10220" yWindow="29300" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -144,48 +144,21 @@
     <t>u</t>
   </si>
   <si>
-    <t>Mega-Fit Right-Angle Header, Single Row, 5.70mm Pitch, 2 Circuits</t>
-  </si>
-  <si>
     <t>Through-Hole</t>
   </si>
   <si>
-    <t>CN4</t>
-  </si>
-  <si>
-    <t>CN5</t>
-  </si>
-  <si>
     <t>1x2POS</t>
   </si>
   <si>
     <t>CONN HEADER R/A 2POS 2.54MM</t>
   </si>
   <si>
-    <t>CN10,CN11</t>
-  </si>
-  <si>
     <t>CUI Devices</t>
   </si>
   <si>
-    <t>Wurth Elektronik</t>
-  </si>
-  <si>
-    <t>TERM BLOCK 2P HORIZON 2.54MM PCB</t>
-  </si>
-  <si>
-    <t>691210910002</t>
-  </si>
-  <si>
     <t>CN12</t>
   </si>
   <si>
-    <t>Amphenol ICC</t>
-  </si>
-  <si>
-    <t>LD09P13A4GX00LF</t>
-  </si>
-  <si>
     <t>CONN D-SUB PLUG 9POS R/A SLDR</t>
   </si>
   <si>
@@ -300,12 +273,6 @@
     <t>1x18POS</t>
   </si>
   <si>
-    <t>CN2,CN3,CN15</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 3POS 2.54MM</t>
-  </si>
-  <si>
     <t>1x3POS</t>
   </si>
   <si>
@@ -315,9 +282,6 @@
     <t>2x5POS</t>
   </si>
   <si>
-    <t>CN6,CN7,CN8,CN9,CN13,CN14</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -331,6 +295,51 @@
   </si>
   <si>
     <t>SMA</t>
+  </si>
+  <si>
+    <t>705510002</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 3POS 2.54MM</t>
+  </si>
+  <si>
+    <t>CN1</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 4POS 5.7MM</t>
+  </si>
+  <si>
+    <t>2x2POS</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 2POS 5.7MM</t>
+  </si>
+  <si>
+    <t>CN2,CN3,CN4,CN5</t>
+  </si>
+  <si>
+    <t>CN6,CN7,CN8,CN9,CN10,CN11</t>
+  </si>
+  <si>
+    <t>CN13,CN14</t>
+  </si>
+  <si>
+    <t>CN15</t>
+  </si>
+  <si>
+    <t>DLS1XP5AK40X</t>
+  </si>
+  <si>
+    <t>Conec</t>
+  </si>
+  <si>
+    <t>08055C103KAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>C8,C9</t>
   </si>
 </sst>
 </file>
@@ -455,7 +464,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -534,6 +543,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -887,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I37"/>
+  <dimension ref="A2:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -962,25 +974,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C7" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="8">
-        <v>2002411202</v>
+        <v>768250004</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="I7" s="10"/>
     </row>
@@ -989,25 +1001,25 @@
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="8">
-        <v>1719710003</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>69</v>
+        <v>2002411222</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="10"/>
     </row>
@@ -1015,26 +1027,26 @@
       <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="11">
-        <v>1</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="B9" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="7">
+        <v>6</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="12">
-        <v>768250010</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="22" t="s">
+      <c r="E9" s="8">
+        <v>705510001</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>17</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="I9" s="14"/>
     </row>
@@ -1042,26 +1054,26 @@
       <c r="A10" s="7">
         <v>4</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="7">
-        <v>6</v>
-      </c>
-      <c r="D10" s="23" t="s">
+      <c r="B10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8">
-        <v>705530001</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>17</v>
+      <c r="E10" s="12">
+        <v>768250010</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="I10" s="10"/>
     </row>
@@ -1070,25 +1082,25 @@
         <v>5</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="10"/>
     </row>
@@ -1096,26 +1108,26 @@
       <c r="A12" s="7">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>27</v>
+      <c r="B12" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>28</v>
+      <c r="D12" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="10"/>
     </row>
@@ -1124,23 +1136,23 @@
         <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E13" s="8">
         <v>3568</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="10"/>
     </row>
@@ -1149,19 +1161,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C14" s="7">
         <v>7</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>11</v>
@@ -1175,25 +1187,25 @@
       <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>39</v>
+      <c r="B15" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C15" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="19" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="10"/>
@@ -1203,103 +1215,103 @@
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1">
+    <row r="17" spans="1:9">
       <c r="A17" s="7">
         <v>11</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="11">
-        <v>2</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="B17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1">
       <c r="A18" s="7">
         <v>12</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="10" t="s">
+      <c r="B18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="10"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7">
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>57</v>
+        <v>44</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>10</v>
@@ -1311,25 +1323,25 @@
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I20" s="10"/>
     </row>
@@ -1338,25 +1350,25 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C21" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="10"/>
     </row>
@@ -1365,81 +1377,108 @@
         <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="7">
+        <v>17</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="7">
         <v>1</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="19" t="s">
+      <c r="D23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="25" t="s">
+      <c r="I23" s="10"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" s="2" customFormat="1">
-      <c r="A27" s="26" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" s="2" customFormat="1">
+      <c r="A28" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-    </row>
-    <row r="37" spans="8:8">
-      <c r="H37" s="3" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+    </row>
+    <row r="38" spans="8:8">
+      <c r="H38" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A28:I28"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A25" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A25:I25" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A26" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A26:I26" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
finished first draft of schematic with Boron
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D3DC74-58AD-1E47-9236-83E176C978E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C9ACBD-BEFF-2943-B03A-897AFCCE7D02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -174,9 +174,6 @@
     <t>FUSE HOLDER BLADE 500V 30A PCB</t>
   </si>
   <si>
-    <t>C1,C2,C3,C4,C5,C6,C7</t>
-  </si>
-  <si>
     <t>AVX Corporation</t>
   </si>
   <si>
@@ -249,30 +246,6 @@
     <t>H1</t>
   </si>
   <si>
-    <t>Sullins Connector Solutions</t>
-  </si>
-  <si>
-    <t>PPPC091LFBN-RC</t>
-  </si>
-  <si>
-    <t>CONN HDR 9POS 0.1 GOLD PCB</t>
-  </si>
-  <si>
-    <t>1x9POS</t>
-  </si>
-  <si>
-    <t>H2,H3</t>
-  </si>
-  <si>
-    <t>PPTC181LFBN-RC</t>
-  </si>
-  <si>
-    <t>CONN HDR 18POS 0.1 TIN PCB</t>
-  </si>
-  <si>
-    <t>1x18POS</t>
-  </si>
-  <si>
     <t>1x3POS</t>
   </si>
   <si>
@@ -327,9 +300,6 @@
     <t>CN15</t>
   </si>
   <si>
-    <t>DLS1XP5AK40X</t>
-  </si>
-  <si>
     <t>Conec</t>
   </si>
   <si>
@@ -339,7 +309,58 @@
     <t>CAP CER 10000PF 50V X7R 0805</t>
   </si>
   <si>
-    <t>C8,C9</t>
+    <t>C1,C2,C3,C4,C5,C6,C7,C8</t>
+  </si>
+  <si>
+    <t>C9,C10</t>
+  </si>
+  <si>
+    <t>C11,C12</t>
+  </si>
+  <si>
+    <t>22pF Ceramic Caps</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>10uF Tantalum Cap</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>47uF Electrolytic Cap</t>
+  </si>
+  <si>
+    <t>1x8 Female Header</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>1x16 Female Header</t>
+  </si>
+  <si>
+    <t>1x12 Female Header</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>MCP2515</t>
+  </si>
+  <si>
+    <t>18-SOIC</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>10k Resistor</t>
   </si>
 </sst>
 </file>
@@ -532,6 +553,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -543,9 +567,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -899,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I38"/>
+  <dimension ref="A2:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -920,25 +941,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="D2" s="27" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="D2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -974,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -986,10 +1007,10 @@
         <v>768250004</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>16</v>
@@ -1001,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C8" s="7">
         <v>4</v>
@@ -1013,7 +1034,7 @@
         <v>2002411222</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>17</v>
@@ -1028,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7">
         <v>6</v>
@@ -1067,10 +1088,10 @@
         <v>768250010</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>16</v>
@@ -1082,7 +1103,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
@@ -1091,13 +1112,13 @@
         <v>12</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>16</v>
@@ -1109,16 +1130,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>21</v>
@@ -1161,19 +1182,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="7">
+        <v>8</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7">
-        <v>7</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>11</v>
@@ -1188,21 +1209,21 @@
         <v>9</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7">
         <v>2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="25" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="19" t="s">
@@ -1214,104 +1235,80 @@
       <c r="A16" s="7">
         <v>10</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>30</v>
+      <c r="B16" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="7">
         <v>11</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>34</v>
+      <c r="B17" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1">
+    <row r="18" spans="1:9">
       <c r="A18" s="7">
         <v>12</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="11">
-        <v>2</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="14"/>
+      <c r="B18" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7">
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>10</v>
@@ -1323,26 +1320,20 @@
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>48</v>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9">
@@ -1350,135 +1341,271 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" s="1" customFormat="1">
       <c r="A22" s="7">
         <v>16</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="11">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="10"/>
+      <c r="D22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="7">
         <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C23" s="7">
         <v>1</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>65</v>
+        <v>43</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="10"/>
     </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="7">
+        <v>18</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7">
+        <v>19</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="7">
+        <v>20</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="7">
+        <v>21</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7">
+        <v>22</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="7">
+        <v>23</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" s="2" customFormat="1">
-      <c r="A28" s="26" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1">
+      <c r="A34" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-    </row>
-    <row r="38" spans="8:8">
-      <c r="H38" s="3" t="s">
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="H44" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A34:I34"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A26" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A26:I26" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A34" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A32" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A32:I32" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
finished first draft of schematic for Boron
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C9ACBD-BEFF-2943-B03A-897AFCCE7D02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C09846C-1D3C-D041-A59A-7680E4200D40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>10k Resistor</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>8MHz Crystal Oscillator</t>
   </si>
 </sst>
 </file>
@@ -920,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I44"/>
+  <dimension ref="A2:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1512,7 +1518,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C28" s="7">
         <v>1</v>
@@ -1520,7 +1526,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="10"/>
@@ -1531,81 +1537,100 @@
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="7">
+        <v>24</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="7">
-        <v>1</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G30" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H30" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I29" s="10"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="26" t="s">
+      <c r="I30" s="10"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-    </row>
-    <row r="34" spans="1:9" s="2" customFormat="1">
-      <c r="A34" s="27" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" s="2" customFormat="1">
+      <c r="A35" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="H44" s="3" t="s">
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="H45" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A35:I35"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A34" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A32" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A32:I32" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A33" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A33:I33" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
finished footprint selection, placement, and silkscreen.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C09846C-1D3C-D041-A59A-7680E4200D40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6C8823-A202-C548-B0A2-7575DB80551F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11900" yWindow="5040" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="115">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -309,64 +309,136 @@
     <t>CAP CER 10000PF 50V X7R 0805</t>
   </si>
   <si>
-    <t>C1,C2,C3,C4,C5,C6,C7,C8</t>
-  </si>
-  <si>
     <t>C9,C10</t>
   </si>
   <si>
     <t>C11,C12</t>
   </si>
   <si>
-    <t>22pF Ceramic Caps</t>
-  </si>
-  <si>
     <t>C13</t>
   </si>
   <si>
-    <t>10uF Tantalum Cap</t>
-  </si>
-  <si>
     <t>C14</t>
   </si>
   <si>
-    <t>47uF Electrolytic Cap</t>
-  </si>
-  <si>
-    <t>1x8 Female Header</t>
-  </si>
-  <si>
     <t>H2</t>
   </si>
   <si>
     <t>H3</t>
   </si>
   <si>
-    <t>1x16 Female Header</t>
-  </si>
-  <si>
-    <t>1x12 Female Header</t>
-  </si>
-  <si>
     <t>IC5</t>
   </si>
   <si>
-    <t>MCP2515</t>
-  </si>
-  <si>
     <t>18-SOIC</t>
   </si>
   <si>
     <t>R2</t>
   </si>
   <si>
-    <t>10k Resistor</t>
-  </si>
-  <si>
     <t>Y1</t>
   </si>
   <si>
-    <t>8MHz Crystal Oscillator</t>
+    <t>C1,C2,C3,C4,C5,C6,C7,C8,C15</t>
+  </si>
+  <si>
+    <t>DLS1XP5AK40X</t>
+  </si>
+  <si>
+    <t>CAP CER 22PF 50V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>478-10742-1-ND</t>
+  </si>
+  <si>
+    <t>CAP TANT 10UF 10% 6.3V 1206</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>478-1308-1-ND</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>493-14562-1-ND</t>
+  </si>
+  <si>
+    <t>CAP ALUM 47UF 20% 25V SMD</t>
+  </si>
+  <si>
+    <t>Radial 6.3mm</t>
+  </si>
+  <si>
+    <t>541-4163-1-ND</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>MCP2515T-I/SOCT-ND</t>
+  </si>
+  <si>
+    <t>IC CAN CONTROLLER W/SPI 18SOIC</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>1x16POS</t>
+  </si>
+  <si>
+    <t>1x12POS</t>
+  </si>
+  <si>
+    <t>1x8POS</t>
+  </si>
+  <si>
+    <t>1x6POS</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>CONN HDR 6POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>S7004-ND</t>
+  </si>
+  <si>
+    <t>S7006-ND</t>
+  </si>
+  <si>
+    <t>CONN HDR 8POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>S6100-ND</t>
+  </si>
+  <si>
+    <t>CONN HDR 12POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>CONN HDR 16POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>S7014-ND</t>
+  </si>
+  <si>
+    <t>Raltron Electronics</t>
+  </si>
+  <si>
+    <t>2151-AS-8.000-18-SMD-TRCT-ND</t>
+  </si>
+  <si>
+    <t>CRYSTAL 8.0000MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>HC-49/US</t>
   </si>
 </sst>
 </file>
@@ -491,7 +563,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,6 +645,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -926,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I45"/>
+  <dimension ref="A2:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="A34" sqref="A34:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -997,7 +1072,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="7">
+      <c r="A7" s="30">
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -1024,7 +1099,7 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7">
+      <c r="A8" s="30">
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -1051,7 +1126,7 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
-      <c r="A9" s="7">
+      <c r="A9" s="30">
         <v>3</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -1078,7 +1153,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="7">
+      <c r="A10" s="30">
         <v>4</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -1105,7 +1180,7 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="7">
+      <c r="A11" s="30">
         <v>5</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -1132,7 +1207,7 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="7">
+      <c r="A12" s="30">
         <v>6</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -1145,7 +1220,7 @@
         <v>68</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>21</v>
@@ -1159,7 +1234,7 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="7">
+      <c r="A13" s="30">
         <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1184,14 +1259,14 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="7">
+      <c r="A14" s="30">
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C14" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>26</v>
@@ -1211,11 +1286,11 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="7">
+      <c r="A15" s="30">
         <v>9</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="7">
         <v>2</v>
@@ -1238,64 +1313,88 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="7">
+      <c r="A16" s="30">
         <v>10</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7">
         <v>2</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="F16" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="30">
+        <v>11</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="30">
+        <v>12</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="7">
-        <v>11</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="7">
-        <v>12</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>77</v>
-      </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="F18" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="19"/>
+        <v>90</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="7">
+      <c r="A19" s="30">
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1322,28 +1421,34 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="7">
+      <c r="A20" s="30">
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F20" s="8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="10"/>
+      <c r="H20" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="7">
+      <c r="A21" s="30">
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1370,7 +1475,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1">
-      <c r="A22" s="7">
+      <c r="A22" s="30">
         <v>16</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -1397,7 +1502,7 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="7">
+      <c r="A23" s="30">
         <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1424,7 +1529,7 @@
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="7">
+      <c r="A24" s="30">
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -1451,28 +1556,34 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="7">
+      <c r="A25" s="30">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="23" t="s">
+        <v>94</v>
+      </c>
       <c r="E25" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="9"/>
+        <v>95</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="G25" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="7">
+      <c r="A26" s="30">
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -1481,156 +1592,211 @@
       <c r="C26" s="7">
         <v>1</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="D26" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="F26" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="15"/>
+        <v>109</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>98</v>
+      </c>
       <c r="H26" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="7">
+      <c r="A27" s="30">
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" s="15"/>
+      <c r="D27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>99</v>
+      </c>
       <c r="H27" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="7">
-        <v>22</v>
+      <c r="A28" s="30">
+        <v>23</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C28" s="7">
         <v>1</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="10"/>
+      <c r="D28" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="7">
-        <v>23</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>81</v>
+      <c r="A29" s="30">
+        <v>23.363636363636399</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>97</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="10"/>
+      <c r="D29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="7">
-        <v>24</v>
+      <c r="A30" s="30">
+        <v>24.409090909090899</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="C30" s="7">
         <v>1</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>57</v>
+        <v>112</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>114</v>
       </c>
       <c r="H30" s="19" t="s">
         <v>10</v>
       </c>
       <c r="I30" s="10"/>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="26" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31" s="30">
+        <v>25.454545454545499</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-    </row>
-    <row r="35" spans="1:9" s="2" customFormat="1">
-      <c r="A35" s="27" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="1:9" s="2" customFormat="1">
+      <c r="A36" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="H45" s="3" t="s">
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="H46" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A36:I36"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A33" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A33:I33" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A34" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A34:I34" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
updated PCB to fix two errors: TX/RX were switched on DB9 jack, and SPI was not connected to MAX31855 ICs
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6C8823-A202-C548-B0A2-7575DB80551F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3FC711-7EF0-3B4B-98D3-6BC24AB9CBEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11900" yWindow="5040" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>CN12</t>
   </si>
   <si>
-    <t>CONN D-SUB PLUG 9POS R/A SLDR</t>
-  </si>
-  <si>
     <t>D-SUB 9POS</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>C1,C2,C3,C4,C5,C6,C7,C8,C15</t>
   </si>
   <si>
-    <t>DLS1XP5AK40X</t>
-  </si>
-  <si>
     <t>CAP CER 22PF 50V C0G/NP0 0805</t>
   </si>
   <si>
@@ -439,6 +433,12 @@
   </si>
   <si>
     <t>HC-49/US</t>
+  </si>
+  <si>
+    <t>DLS1XS5AK40X</t>
+  </si>
+  <si>
+    <t>CONN D-SUB RCPT 9POS R/A SLDR</t>
   </si>
 </sst>
 </file>
@@ -634,6 +634,9 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -645,9 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1004,7 +1004,7 @@
   <dimension ref="A2:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:I34"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1022,25 +1022,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="D2" s="28" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="D2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1072,11 +1072,11 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="30">
+      <c r="A7" s="26">
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1088,10 +1088,10 @@
         <v>768250004</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>62</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>16</v>
@@ -1099,11 +1099,11 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="30">
+      <c r="A8" s="26">
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="7">
         <v>4</v>
@@ -1115,7 +1115,7 @@
         <v>2002411222</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>17</v>
@@ -1126,11 +1126,11 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
-      <c r="A9" s="30">
+      <c r="A9" s="26">
         <v>3</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="7">
         <v>6</v>
@@ -1153,7 +1153,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="30">
+      <c r="A10" s="26">
         <v>4</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -1169,10 +1169,10 @@
         <v>768250010</v>
       </c>
       <c r="F10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>52</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>16</v>
@@ -1180,11 +1180,11 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="30">
+      <c r="A11" s="26">
         <v>5</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
@@ -1193,13 +1193,13 @@
         <v>12</v>
       </c>
       <c r="E11" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="G11" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>16</v>
@@ -1207,26 +1207,26 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="30">
+      <c r="A12" s="26">
         <v>6</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>68</v>
-      </c>
       <c r="E12" s="8" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>16</v>
@@ -1234,23 +1234,23 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="30">
+      <c r="A13" s="26">
         <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="E13" s="8">
         <v>3568</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="10" t="s">
@@ -1259,23 +1259,23 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="30">
+      <c r="A14" s="26">
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="7">
         <v>9</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>11</v>
@@ -1286,23 +1286,23 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="30">
+      <c r="A15" s="26">
         <v>9</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="7">
         <v>2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="G15" s="25" t="s">
         <v>11</v>
@@ -1313,23 +1313,23 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="30">
+      <c r="A16" s="26">
         <v>10</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="7">
         <v>2</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G16" s="25" t="s">
         <v>11</v>
@@ -1340,26 +1340,26 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="30">
+      <c r="A17" s="26">
         <v>11</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>84</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>86</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>10</v>
@@ -1367,26 +1367,26 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="30">
+      <c r="A18" s="26">
         <v>12</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
       <c r="D18" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="G18" s="25" t="s">
         <v>89</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>91</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>10</v>
@@ -1394,23 +1394,23 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="30">
+      <c r="A19" s="26">
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>11</v>
@@ -1421,23 +1421,23 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="30">
+      <c r="A20" s="26">
         <v>14</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>11</v>
@@ -1448,11 +1448,11 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="30">
+      <c r="A21" s="26">
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
@@ -1461,10 +1461,10 @@
         <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>17</v>
@@ -1475,26 +1475,26 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1">
-      <c r="A22" s="30">
+      <c r="A22" s="26">
         <v>16</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="11">
         <v>2</v>
       </c>
       <c r="D22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="G22" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="H22" s="14" t="s">
         <v>10</v>
@@ -1502,26 +1502,26 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="30">
+      <c r="A23" s="26">
         <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="7">
-        <v>1</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="G23" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>10</v>
@@ -1529,26 +1529,26 @@
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="30">
+      <c r="A24" s="26">
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="7">
-        <v>1</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>10</v>
@@ -1556,26 +1556,26 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="30">
+      <c r="A25" s="26">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="C25" s="7">
-        <v>1</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>78</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>10</v>
@@ -1583,26 +1583,26 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="30">
+      <c r="A26" s="26">
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7">
         <v>1</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>16</v>
@@ -1610,26 +1610,26 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="30">
+      <c r="A27" s="26">
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>16</v>
@@ -1637,26 +1637,26 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="30">
+      <c r="A28" s="26">
         <v>23</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="7">
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>16</v>
@@ -1664,26 +1664,26 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="30">
+      <c r="A29" s="26">
         <v>23.363636363636399</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="F29" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H29" s="10" t="s">
         <v>16</v>
@@ -1691,26 +1691,26 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="30">
+      <c r="A30" s="26">
         <v>24.409090909090899</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="7">
         <v>1</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="G30" s="25" t="s">
         <v>112</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>114</v>
       </c>
       <c r="H30" s="19" t="s">
         <v>10</v>
@@ -1718,26 +1718,26 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="30">
+      <c r="A31" s="26">
         <v>25.454545454545499</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="F31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="15" t="s">
         <v>56</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>10</v>
@@ -1745,17 +1745,17 @@
       <c r="I31" s="10"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="17"/>
@@ -1769,17 +1769,17 @@
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
     </row>
     <row r="46" spans="1:9">
       <c r="H46" s="3" t="s">

</xml_diff>

<commit_message>
made some final changes to PCB and BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3FC711-7EF0-3B4B-98D3-6BC24AB9CBEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0886D8-5BA7-0D48-B5F7-405004B7DE73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="5040" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="137">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -381,9 +381,6 @@
     <t>IC CAN CONTROLLER W/SPI 18SOIC</t>
   </si>
   <si>
-    <t>H4</t>
-  </si>
-  <si>
     <t>1x16POS</t>
   </si>
   <si>
@@ -393,18 +390,9 @@
     <t>1x8POS</t>
   </si>
   <si>
-    <t>1x6POS</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>CONN HDR 6POS 0.1 TIN PCB</t>
-  </si>
-  <si>
-    <t>S7004-ND</t>
-  </si>
-  <si>
     <t>S7006-ND</t>
   </si>
   <si>
@@ -439,6 +427,84 @@
   </si>
   <si>
     <t>CONN D-SUB RCPT 9POS R/A SLDR</t>
+  </si>
+  <si>
+    <t>DigiKey URL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0768250004/5639612?s=N4IgTCBcDaIOwDYAcYCsAGTAWEBdAvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/2002411222/10709049?s=N4IgTCBcDa4AxzAFgIwrBkBdAvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0705510001/2421652?s=N4IgTCBcDaIOwAYCsSCMCOpAXQL5A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0768250010/5639615?s=N4IgTCBcDaIOwDYAcYCsAGdBGdIC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0705510002/3468756?s=N4IgTCBcDaIOwAYCsSCMCMQLoF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/conec/DLS1XS5AK40X/3534022?s=N4IgTCBcDaICIBkDKBGAGkgrAQQNIBYAGNEAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/3568/2137306</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/avx-corporation/08055C104KAT2A/563505?s=N4IgTCBcDaIAwA44FZkGECMcAsBpAggCpj4gC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/avx-corporation/08055C103KAT2A/563493?s=N4IgTCBcDaIAwA44FZkGECMcDMBpAggCpj4gC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/avx-corporation/08055A220JAT2A/563418?s=N4IgTCBcDaICwHYAcBaAjAZgAyrSgcgCIgC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/avx-corporation/TAJA106K006SNJ/7536093?s=N4IgTCBcDaICwHYAcBaAjABgXM6UDkAREAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/nichicon/UWR1E470MCL1GB/4995567?s=N4IgTCBcDaICwE4DMBaAjHArANjOlAcgCIgC6AvkA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW0805120RFKEAC/7922316?s=N4IgTCBcDaIMICU4HUAMAOVBWAjGVCAYgNICiAgnCALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW080510K0JNEAC/7928585?s=N4IgTCBcDaIKwBYCMBaZA2AzC1A5AIiALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/cui-devices/DS01-254-L-01BE/11310875?s=N4IgTCBcDaICIGUAMBGAtGArAFjQGTVQCEBREAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/maxim-integrated/MAX31855KASA-T/2591213?s=N4IgTCBcDaILIEEAaBmAjADgKxYNIIGUEBqAFRAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/TCAN332DR/5823563?s=N4IgTCBcDaICoGECCA5AzGsARASiAugL5A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/MAX3232CPWR/484760</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/microchip-technology/MCP2515T-I-SO/593681?s=N4IgTCBcDaILIGEAKYCsBGVAVAtASQHoBlAeQVwDkAREAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC161LFBN-RC/810154?s=N4IgTCBcDaIMoHYAMBGALAWgHIBEQF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC121LFBN-RC/807231?s=N4IgTCBcDaIMoDYCMAGFBaAcgERAXQF8g</t>
+  </si>
+  <si>
+    <t>1 of 2 Headers for PCB component Particle_Boron</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC081LFBN-RC/810147?s=N4IgTCBcDaIMoHYAMSBsBaAcgERAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/raltron-electronics/AS-8-000-18-SMD-TR/10271835?s=N4IgTCBcDa4IwFY4FoCCBlZAOAdABgOTi2XQFkARZAFQCUBha5AOQpAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/S1A-13-F/749977</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I46"/>
+  <dimension ref="A2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1017,11 +1083,12 @@
     <col min="6" max="6" width="54" style="3" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="3"/>
+    <col min="9" max="9" width="41.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="138.1640625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1">
+    <row r="2" spans="1:10" ht="19.5" customHeight="1">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="D2" s="29" t="s">
@@ -1030,19 +1097,19 @@
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
     </row>
-    <row r="6" spans="1:9" ht="28.5" customHeight="1">
+    <row r="6" spans="1:10" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1070,8 +1137,11 @@
       <c r="I6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="26">
         <v>1</v>
       </c>
@@ -1097,8 +1167,11 @@
         <v>16</v>
       </c>
       <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="26">
         <v>2</v>
       </c>
@@ -1124,8 +1197,11 @@
         <v>16</v>
       </c>
       <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1">
+      <c r="J8" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1">
       <c r="A9" s="26">
         <v>3</v>
       </c>
@@ -1151,8 +1227,11 @@
         <v>16</v>
       </c>
       <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="26">
         <v>4</v>
       </c>
@@ -1178,8 +1257,11 @@
         <v>16</v>
       </c>
       <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="26">
         <v>5</v>
       </c>
@@ -1205,8 +1287,11 @@
         <v>16</v>
       </c>
       <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="26">
         <v>6</v>
       </c>
@@ -1220,10 +1305,10 @@
         <v>67</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>21</v>
@@ -1232,8 +1317,11 @@
         <v>16</v>
       </c>
       <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="26">
         <v>7</v>
       </c>
@@ -1257,8 +1345,11 @@
         <v>16</v>
       </c>
       <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="26">
         <v>8</v>
       </c>
@@ -1284,8 +1375,11 @@
         <v>10</v>
       </c>
       <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="26">
         <v>9</v>
       </c>
@@ -1311,8 +1405,11 @@
         <v>10</v>
       </c>
       <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="26">
         <v>10</v>
       </c>
@@ -1338,8 +1435,11 @@
         <v>10</v>
       </c>
       <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="26">
         <v>11</v>
       </c>
@@ -1365,8 +1465,11 @@
         <v>10</v>
       </c>
       <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="26">
         <v>12</v>
       </c>
@@ -1392,8 +1495,11 @@
         <v>10</v>
       </c>
       <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="26">
         <v>13</v>
       </c>
@@ -1419,8 +1525,11 @@
         <v>10</v>
       </c>
       <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="26">
         <v>14</v>
       </c>
@@ -1446,8 +1555,11 @@
         <v>10</v>
       </c>
       <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="26">
         <v>15</v>
       </c>
@@ -1473,8 +1585,11 @@
         <v>16</v>
       </c>
       <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1">
+      <c r="J21" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1">
       <c r="A22" s="26">
         <v>16</v>
       </c>
@@ -1500,8 +1615,11 @@
         <v>10</v>
       </c>
       <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="26">
         <v>17</v>
       </c>
@@ -1527,8 +1645,11 @@
         <v>10</v>
       </c>
       <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="26">
         <v>18</v>
       </c>
@@ -1554,8 +1675,11 @@
         <v>10</v>
       </c>
       <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="26">
         <v>19</v>
       </c>
@@ -1581,8 +1705,11 @@
         <v>10</v>
       </c>
       <c r="I25" s="10"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="26">
         <v>20</v>
       </c>
@@ -1593,23 +1720,28 @@
         <v>1</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="I26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="26">
         <v>21</v>
       </c>
@@ -1620,23 +1752,28 @@
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="I27" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="26">
         <v>23</v>
       </c>
@@ -1647,156 +1784,138 @@
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>104</v>
-      </c>
       <c r="G28" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="10"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="26">
-        <v>23.363636363636399</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>95</v>
+        <v>24.409090909090899</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>101</v>
+        <v>106</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>16</v>
+        <v>108</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>10</v>
       </c>
       <c r="I29" s="10"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="26">
-        <v>24.409090909090899</v>
+        <v>25.454545454545499</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C30" s="7">
         <v>1</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>112</v>
+        <v>54</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="H30" s="19" t="s">
         <v>10</v>
       </c>
       <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="26">
-        <v>25.454545454545499</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I31" s="10"/>
+      <c r="J30" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-    </row>
-    <row r="36" spans="1:9" s="2" customFormat="1">
-      <c r="A36" s="28" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" s="2" customFormat="1">
+      <c r="A35" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="H46" s="3" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="H45" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A35:I35"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A34" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A34:I34" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A33" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A33:I33" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
revert before everything was messed up
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0886D8-5BA7-0D48-B5F7-405004B7DE73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BEF3DF-E7CE-6848-8CB8-8A6B81E159F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10220" yWindow="29300" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="160">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -506,12 +506,81 @@
   <si>
     <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/S1A-13-F/749977</t>
   </si>
+  <si>
+    <t>R3, R5</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>LTST-C170KRKT</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR SMD</t>
+  </si>
+  <si>
+    <t>LTST-C171KGKT</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR SMD</t>
+  </si>
+  <si>
+    <t>LTST-C170AKT</t>
+  </si>
+  <si>
+    <t>LED ORANGE CLEAR SMD</t>
+  </si>
+  <si>
+    <t>LTST-C170TBKT</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR SMD</t>
+  </si>
+  <si>
+    <t>0806</t>
+  </si>
+  <si>
+    <t>CRCW080568R0JNEA</t>
+  </si>
+  <si>
+    <t>RES SMD 68 OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>CRCW08054R70JNEA</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7 OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>CRCW0805560RJNEA</t>
+  </si>
+  <si>
+    <t>RES SMD 560 OHM 5% 1/8W 0805</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +644,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -629,7 +709,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -714,6 +794,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1067,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J45"/>
+  <dimension ref="A2:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1564,149 +1653,143 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="C21" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>34</v>
+        <v>153</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>16</v>
+        <v>154</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>10</v>
       </c>
       <c r="I21" s="10"/>
-      <c r="J21" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="1" customFormat="1">
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="26">
         <v>16</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="11">
-        <v>2</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="14" t="s">
+      <c r="B22" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14" t="s">
-        <v>127</v>
-      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="26">
         <v>17</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>40</v>
+      <c r="B23" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="C23" s="7">
         <v>1</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="10"/>
-      <c r="J23" s="10" t="s">
-        <v>128</v>
-      </c>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="26">
         <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C24" s="7">
         <v>1</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1">
       <c r="A25" s="26">
         <v>19</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="7">
-        <v>1</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="19" t="s">
+      <c r="B25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="11">
+        <v>2</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10" t="s">
-        <v>130</v>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1714,31 +1797,29 @@
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="7">
         <v>1</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>95</v>
+        <v>43</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>133</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I26" s="10"/>
       <c r="J26" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1746,176 +1827,381 @@
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>96</v>
+        <v>45</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>133</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I27" s="10"/>
       <c r="J27" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="26">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="7">
         <v>1</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>98</v>
+      <c r="D28" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>16</v>
+        <v>93</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>10</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26">
-        <v>24.409090909090899</v>
+        <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="10"/>
+        <v>95</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>133</v>
+      </c>
       <c r="J29" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="26">
-        <v>25.454545454545499</v>
+        <v>24</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="26">
+        <v>25</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="26">
+        <v>26</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="26">
+        <v>27</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="7">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G33" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H33" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10" t="s">
+      <c r="I33" s="10"/>
+      <c r="J33" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="27" t="s">
+    <row r="34" spans="1:10">
+      <c r="A34" s="26">
+        <v>28</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="26">
+        <v>29</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="26">
+        <v>30</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="26">
+        <v>31</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-    </row>
-    <row r="35" spans="1:9" s="2" customFormat="1">
-      <c r="A35" s="28" t="s">
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" s="2" customFormat="1">
+      <c r="A41" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="H45" s="3" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+    </row>
+    <row r="51" spans="8:8">
+      <c r="H51" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="A41:I41"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A33" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A33:I33" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A39" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A39:I39" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
added JLPCB gerber files
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BEF3DF-E7CE-6848-8CB8-8A6B81E159F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12CDA87-57DC-034D-A891-A20B939EEC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="29300" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14960" yWindow="-28300" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="161">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -366,12 +366,6 @@
     <t>Radial 6.3mm</t>
   </si>
   <si>
-    <t>541-4163-1-ND</t>
-  </si>
-  <si>
-    <t>RES 10K OHM 5% 1/8W 0805</t>
-  </si>
-  <si>
     <t>Microchip Technology</t>
   </si>
   <si>
@@ -507,12 +501,6 @@
     <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/S1A-13-F/749977</t>
   </si>
   <si>
-    <t>R3, R5</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -528,52 +516,67 @@
     <t>Lite-On Inc.</t>
   </si>
   <si>
-    <t>LTST-C170KRKT</t>
-  </si>
-  <si>
-    <t>LED RED CLEAR SMD</t>
-  </si>
-  <si>
-    <t>LTST-C171KGKT</t>
-  </si>
-  <si>
-    <t>LED GREEN CLEAR SMD</t>
-  </si>
-  <si>
-    <t>LTST-C170AKT</t>
-  </si>
-  <si>
     <t>LED ORANGE CLEAR SMD</t>
   </si>
   <si>
-    <t>LTST-C170TBKT</t>
-  </si>
-  <si>
-    <t>LED BLUE CLEAR SMD</t>
-  </si>
-  <si>
-    <t>0806</t>
-  </si>
-  <si>
     <t>CRCW080568R0JNEA</t>
   </si>
   <si>
     <t>RES SMD 68 OHM 5% 1/8W 0805</t>
   </si>
   <si>
-    <t>CRCW08054R70JNEA</t>
-  </si>
-  <si>
-    <t>RES SMD 4.7 OHM 5% 1/8W 0805</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
-    <t>CRCW0805560RJNEA</t>
-  </si>
-  <si>
-    <t>RES SMD 560 OHM 5% 1/8W 0805</t>
+    <t>LTST-C170KFKT</t>
+  </si>
+  <si>
+    <t>Würth Elektronik</t>
+  </si>
+  <si>
+    <t>150080BS75000</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>150080GS75000</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>150080RS75000</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>RES SMD 5.6 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>CRCW08055R60FKEA</t>
+  </si>
+  <si>
+    <t>RCS0805560RJNEA</t>
+  </si>
+  <si>
+    <t>RES SMD 560 OHM 5% 0.4W 0805</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD10K0</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/4W 0805</t>
   </si>
 </sst>
 </file>
@@ -783,6 +786,15 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -794,15 +806,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1158,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1178,25 +1181,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="D2" s="29" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="D2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1227,7 +1230,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1257,7 +1260,7 @@
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1287,7 +1290,7 @@
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1">
@@ -1317,7 +1320,7 @@
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1347,7 +1350,7 @@
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1377,7 +1380,7 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1394,10 +1397,10 @@
         <v>67</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>21</v>
@@ -1407,7 +1410,7 @@
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1435,7 +1438,7 @@
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1465,7 +1468,7 @@
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1495,7 +1498,7 @@
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1525,7 +1528,7 @@
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1555,7 +1558,7 @@
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1585,7 +1588,7 @@
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1615,7 +1618,7 @@
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1629,13 +1632,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>29</v>
+        <v>158</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>11</v>
@@ -1645,27 +1648,27 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26">
         <v>15</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>137</v>
+      <c r="B21" s="23" t="s">
+        <v>152</v>
       </c>
       <c r="C21" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>11</v>
@@ -1680,8 +1683,8 @@
       <c r="A22" s="26">
         <v>16</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>138</v>
+      <c r="B22" s="23" t="s">
+        <v>153</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
@@ -1693,7 +1696,7 @@
         <v>155</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>11</v>
@@ -1709,7 +1712,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C23" s="7">
         <v>1</v>
@@ -1718,10 +1721,10 @@
         <v>29</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>11</v>
@@ -1759,7 +1762,7 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1">
@@ -1789,7 +1792,7 @@
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1819,7 +1822,7 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1849,7 +1852,7 @@
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1863,13 +1866,13 @@
         <v>1</v>
       </c>
       <c r="D28" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>77</v>
@@ -1879,7 +1882,7 @@
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1893,25 +1896,25 @@
         <v>1</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H29" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1925,25 +1928,25 @@
         <v>1</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1957,23 +1960,23 @@
         <v>1</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>100</v>
-      </c>
       <c r="G31" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1987,23 +1990,23 @@
         <v>1</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="G32" s="25" t="s">
         <v>106</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>108</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>10</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2033,7 +2036,7 @@
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2041,19 +2044,19 @@
         <v>28</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C34" s="7">
         <v>1</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>145</v>
+        <v>151</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>150</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>11</v>
@@ -2069,19 +2072,19 @@
         <v>29</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G35" s="25" t="s">
         <v>11</v>
@@ -2096,20 +2099,20 @@
       <c r="A36" s="26">
         <v>30</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>141</v>
+      <c r="B36" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="C36" s="7">
         <v>1</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="G36" s="25" t="s">
         <v>11</v>
@@ -2125,41 +2128,41 @@
         <v>31</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F37" s="33" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>140</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="H37" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="17"/>
@@ -2173,17 +2176,17 @@
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:10" s="2" customFormat="1">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
     </row>
     <row r="51" spans="8:8">
       <c r="H51" s="3" t="s">

</xml_diff>

<commit_message>
updated BOM with some missing items + external connectors
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/github/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12CDA87-57DC-034D-A891-A20B939EEC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FCBACC-4A90-7F46-8E5B-1FE0886ED2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="-28300" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="199">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -465,9 +465,6 @@
     <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW0805120RFKEAC/7922316?s=N4IgTCBcDaIMICU4HUAMAOVBWAjGVCAYgNICiAgnCALoC%2BQA</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW080510K0JNEAC/7928585?s=N4IgTCBcDaIKwBYCMBaZA2AzC1A5AIiALoC%2BQA</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/cui-devices/DS01-254-L-01BE/11310875?s=N4IgTCBcDaICIGUAMBGAtGArAFjQGTVQCEBREAXQF8g</t>
   </si>
   <si>
@@ -577,6 +574,123 @@
   </si>
   <si>
     <t>RES 10K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>Wurth Elektronik</t>
+  </si>
+  <si>
+    <t>PLASTIC SPACER STUD METRIC THREA</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/970110365/9488701</t>
+  </si>
+  <si>
+    <t>M3x11mm Nylon Spacer (for GPS)</t>
+  </si>
+  <si>
+    <t>PAN HEAD SCREW_M3 X 6MM CROSS SL</t>
+  </si>
+  <si>
+    <t>M3x6mm Nylon Screw (for GPS)</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
+    <t>0297025.WXNV</t>
+  </si>
+  <si>
+    <t>FUSE AUTO 25A 32VDC BLADE MINI</t>
+  </si>
+  <si>
+    <t>ATM (Auto Mini)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/littelfuse-inc/0297025-WXNV/146602</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/97790603111/10056387</t>
+  </si>
+  <si>
+    <t>Wire Connectors:</t>
+  </si>
+  <si>
+    <t>CONN RCPT HSG 4POS 5.70MM</t>
+  </si>
+  <si>
+    <t>MEGA-FIT RECEP HSG SR TOPL 2CKT</t>
+  </si>
+  <si>
+    <t>2x1POS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/2004561212/10709200</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/1716920104/WM10386-ND/4515272?itemSeq=377049648</t>
+  </si>
+  <si>
+    <t>CONN RCPT HSG 10POS 5.70MM</t>
+  </si>
+  <si>
+    <t>5x2POS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/1716920110/4515275</t>
+  </si>
+  <si>
+    <t>CONN HSG 2POS .100 SINGLE VER DCONN HOUSING 2POS .100 W/LATCH</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0050579402/115029</t>
+  </si>
+  <si>
+    <t>CONN HSG 3POS .100 SINGLE VER N</t>
+  </si>
+  <si>
+    <t>3x1POS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0050579703/2731437</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 12AWG CRIMP TIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0768230322/5639624</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 22-24AWG CRIMP TIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/molex/0016020086/467788</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/lite-on-inc/LTST-C170KFKT/386775?s=N4IgTCBcDaIDIBUDKCC0BhAjAdgAwGkAxfBEAXQF8g</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/150080BS75000/4489912?s=N4IgTCBcDaIIwFYAMSAcSBCBlA7MlIAugL5A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/150080GS75000/4489915?s=N4IgTCBcDaIIwFYAMSAcSDiBlA7MlIAugL5A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/150080RS75000/4489918?s=N4IgTCBcDaIIwFYAMSAcSBKBlA7MlIAugL5A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/RCS0805560RJNEA/5869655?s=N4IgTCBcDaIEoGEDKAGAHCgrJgbCuAUgHICiAgiALoC%2BQA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW08055R60FKEA/1961736</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW080568R0JNEA/1175170</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RNCP0805FTD10K0/2240262?s=N4IgTCBcDaIEoDkDCAFADADjQVgGIBUARARjQGk0QBdAXyA</t>
   </si>
 </sst>
 </file>
@@ -679,7 +793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -702,6 +816,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -712,7 +863,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -806,6 +957,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1159,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J51"/>
+  <dimension ref="A2:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:F24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1632,13 +1795,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>11</v>
@@ -1648,7 +1811,7 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1656,7 +1819,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
@@ -1665,10 +1828,10 @@
         <v>29</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>142</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>11</v>
@@ -1677,14 +1840,16 @@
         <v>10</v>
       </c>
       <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="J21" s="10" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="26">
         <v>16</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
@@ -1693,10 +1858,10 @@
         <v>29</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>11</v>
@@ -1705,14 +1870,16 @@
         <v>10</v>
       </c>
       <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="J22" s="10" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="26">
         <v>17</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" s="7">
         <v>1</v>
@@ -1721,10 +1888,10 @@
         <v>29</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>11</v>
@@ -1733,7 +1900,9 @@
         <v>10</v>
       </c>
       <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="J23" s="10" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="26">
@@ -1762,7 +1931,7 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1">
@@ -1792,7 +1961,7 @@
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1822,7 +1991,7 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1852,7 +2021,7 @@
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1882,7 +2051,7 @@
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1911,10 +2080,10 @@
         <v>16</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1943,10 +2112,10 @@
         <v>16</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1976,7 +2145,7 @@
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2006,7 +2175,7 @@
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2036,7 +2205,7 @@
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2044,19 +2213,19 @@
         <v>28</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="7">
         <v>1</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>11</v>
@@ -2065,26 +2234,28 @@
         <v>10</v>
       </c>
       <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
+      <c r="J34" s="10" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="26">
         <v>29</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E35" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="G35" s="25" t="s">
         <v>11</v>
@@ -2093,26 +2264,28 @@
         <v>10</v>
       </c>
       <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
+      <c r="J35" s="10" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="26">
         <v>30</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C36" s="7">
         <v>1</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="F36" s="27" t="s">
         <v>146</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>147</v>
       </c>
       <c r="G36" s="25" t="s">
         <v>11</v>
@@ -2121,26 +2294,28 @@
         <v>10</v>
       </c>
       <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="J36" s="10" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="26">
         <v>31</v>
       </c>
       <c r="B37" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="7">
-        <v>1</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>140</v>
       </c>
       <c r="G37" s="25" t="s">
         <v>11</v>
@@ -2149,62 +2324,339 @@
         <v>10</v>
       </c>
       <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
+      <c r="J37" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="26">
+        <v>32</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="7">
+        <v>4</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="8">
+        <v>970110365</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="H38" s="19"/>
+      <c r="I38" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="J38" s="37" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="26">
+        <v>33</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="7">
+        <v>4</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" s="8">
+        <v>97790603111</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="H39" s="19"/>
+      <c r="I39" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="J39" s="27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="26">
+        <v>34</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="H40" s="19"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="36"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="26">
+        <v>35</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1716920104</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="19"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="26">
+        <v>36</v>
+      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="7">
+        <v>4</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="8">
+        <v>2004561212</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H43" s="19"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="26">
+        <v>37</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="8">
+        <v>1716920110</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="H44" s="19"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="26">
+        <v>38</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="7">
+        <v>6</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="8">
+        <v>50579402</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="H45" s="19"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="26">
+        <v>39</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="7">
+        <v>2</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="8">
+        <v>50579703</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" s="19"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="26">
+        <v>40</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" s="7">
+        <v>22</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="8">
+        <v>768230322</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="25"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="26">
+        <v>41</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="7">
+        <v>18</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="8">
+        <v>16020086</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="G48" s="25"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-    </row>
-    <row r="41" spans="1:10" s="2" customFormat="1">
-      <c r="A41" s="31" t="s">
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="1:9" s="2" customFormat="1">
+      <c r="A52" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-    </row>
-    <row r="51" spans="8:8">
-      <c r="H51" s="3" t="s">
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="H62" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A41:I41"/>
+  <mergeCells count="5">
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="A52:I52"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A41:J41"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A39" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A39:I39" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A52" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A50" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A50:I50" r:id="rId2" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
Shrinks board and removes GPS. Replaces GPS with Qwiic connector for off-board GPS
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/git/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51662DA-4DD4-AE42-9B46-438C77ECFB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FC2164-D689-1C42-9116-B28293616D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30720" yWindow="-9100" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="233">
   <si>
     <r>
       <rPr>
@@ -216,9 +216,6 @@
     <t>C14</t>
   </si>
   <si>
-    <t>H2</t>
-  </si>
-  <si>
     <t>IC5</t>
   </si>
   <si>
@@ -255,18 +252,9 @@
     <t>1x12POS</t>
   </si>
   <si>
-    <t>1x8POS</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>S7006-ND</t>
-  </si>
-  <si>
-    <t>CONN HDR 8POS 0.1 TIN PCB</t>
-  </si>
-  <si>
     <t>S6100-ND</t>
   </si>
   <si>
@@ -306,9 +294,6 @@
     <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC121LFBN-RC/807231?s=N4IgTCBcDaIMoDYCMAGFBaAcgERAXQF8g</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC081LFBN-RC/810147?s=N4IgTCBcDaIMoHYAMSBsBaAcgERAXQF8g</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/diodes-incorporated/S1A-13-F/749977</t>
   </si>
   <si>
@@ -702,12 +687,6 @@
     <t>Not on PCB:</t>
   </si>
   <si>
-    <t>M3x6mm Screws</t>
-  </si>
-  <si>
-    <t>M3x11mm Standoffs (Threaded F/F)</t>
-  </si>
-  <si>
     <t>QPC02SXGN-RC</t>
   </si>
   <si>
@@ -766,6 +745,54 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/bel-fuse-inc/0679L1000-05/5844030</t>
+  </si>
+  <si>
+    <t>CN8</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/jst-sales-america-inc/SM04B-SRSS-TB-LF-SN/926710</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD R/A 4POS 1MM</t>
+  </si>
+  <si>
+    <t>SM04B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>Particle Industries, Inc.</t>
+  </si>
+  <si>
+    <t>BRN402</t>
+  </si>
+  <si>
+    <t>BORON LTE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/particle-industries-inc/BRN402/9681356</t>
+  </si>
+  <si>
+    <t>SparkFun Electronics</t>
+  </si>
+  <si>
+    <t>GPS-15210</t>
+  </si>
+  <si>
+    <t>SPARKFUN GPS BREAKOUT - CHIP ANT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sparkfun-electronics/GPS-15210/10064422</t>
+  </si>
+  <si>
+    <t>PRT-17257</t>
+  </si>
+  <si>
+    <t>FLEXIBLE QWIIC CABLE - 500MM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sparkfun-electronics/PRT-17257/13629026</t>
   </si>
 </sst>
 </file>
@@ -941,15 +968,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -998,6 +1016,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1351,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H73"/>
+  <dimension ref="A2:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1371,13 +1398,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A2" s="16"/>
+      <c r="A2" s="33"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="16"/>
+      <c r="A3" s="33"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -1410,47 +1437,47 @@
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="18">
+        <v>82</v>
+      </c>
+      <c r="B7" s="15">
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="18">
+        <v>86</v>
+      </c>
+      <c r="B8" s="15">
         <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>15</v>
@@ -1462,24 +1489,24 @@
         <v>7</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="18">
+        <v>90</v>
+      </c>
+      <c r="B9" s="15">
         <v>2</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>8</v>
@@ -1488,24 +1515,24 @@
         <v>7</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="15">
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>8</v>
@@ -1514,66 +1541,66 @@
         <v>7</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="15">
         <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="15">
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="18">
+        <v>101</v>
+      </c>
+      <c r="B13" s="15">
         <v>2</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1585,31 +1612,31 @@
       <c r="E13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="18">
+        <v>102</v>
+      </c>
+      <c r="B14" s="15">
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>14</v>
@@ -1618,414 +1645,414 @@
         <v>11</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="18">
+        <v>110</v>
+      </c>
+      <c r="B15" s="15">
         <v>1</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="18">
+        <v>116</v>
+      </c>
+      <c r="B16" s="15">
         <v>2</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="16" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="23" t="s">
         <v>28</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="15">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="18">
-        <v>1</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="B18" s="15">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F18" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" s="20">
-        <v>1</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>125</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>126</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="20">
+        <v>117</v>
+      </c>
+      <c r="B19" s="17">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="20">
+        <v>123</v>
+      </c>
+      <c r="B20" s="17">
         <v>1</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="20">
+        <v>122</v>
+      </c>
+      <c r="B21" s="17">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>53</v>
+      <c r="F21" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="20">
+        <v>124</v>
+      </c>
+      <c r="B22" s="17">
         <v>1</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>131</v>
+        <v>125</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="23" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="20">
+        <v>128</v>
+      </c>
+      <c r="B23" s="17">
         <v>2</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="18" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="24" t="s">
         <v>21</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>7</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="17">
         <v>1</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="E24" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>42</v>
+      <c r="F24" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="20">
+        <v>40</v>
+      </c>
+      <c r="B25" s="17">
         <v>1</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="20">
+        <v>129</v>
+      </c>
+      <c r="B26" s="17">
         <v>1</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>136</v>
+        <v>130</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="20">
+        <v>135</v>
+      </c>
+      <c r="B27" s="17">
         <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>141</v>
+        <v>103</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>136</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>143</v>
+        <v>137</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="20">
+        <v>140</v>
+      </c>
+      <c r="B28" s="17">
         <v>1</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>147</v>
+        <v>52</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="23" t="s">
         <v>37</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="20">
+        <v>141</v>
+      </c>
+      <c r="B29" s="17">
         <v>1</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>149</v>
+        <v>103</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22" t="s">
-        <v>72</v>
+      <c r="A30" s="19" t="s">
+        <v>67</v>
       </c>
       <c r="B30" s="11">
         <v>1</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>159</v>
+      <c r="C30" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>154</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>8</v>
@@ -2033,25 +2060,25 @@
       <c r="G30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="22" t="s">
-        <v>154</v>
+      <c r="H30" s="19" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="11">
+        <v>1</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="11">
-        <v>1</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>158</v>
+      <c r="E31" s="19" t="s">
+        <v>153</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>8</v>
@@ -2059,25 +2086,25 @@
       <c r="G31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H31" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="11">
+        <v>1</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="11">
-        <v>1</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>160</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>8</v>
@@ -2085,25 +2112,25 @@
       <c r="G32" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="11">
+        <v>1</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="11">
-        <v>1</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>161</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>8</v>
@@ -2111,573 +2138,607 @@
       <c r="G33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H33" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="19" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
-        <v>162</v>
-      </c>
       <c r="B34" s="11">
         <v>1</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22" t="s">
+      <c r="C34" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="22" t="s">
-        <v>166</v>
+      <c r="H34" s="19" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="17">
         <v>1</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>167</v>
+        <v>75</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" s="23" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1">
       <c r="A36" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="23">
+        <v>42</v>
+      </c>
+      <c r="B36" s="20">
         <v>1</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>170</v>
+        <v>75</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>165</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F36" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F36" s="23" t="s">
         <v>8</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B37" s="20">
+        <v>168</v>
+      </c>
+      <c r="B37" s="17">
         <v>3</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>175</v>
+      <c r="C37" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="22" t="s">
+      <c r="H37" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" s="11">
+        <v>1</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="11">
+        <v>1</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="22" t="s">
+      <c r="D39" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="B38" s="11">
-        <v>1</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="22" t="s">
+      <c r="E39" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="F39" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="F38" s="24" t="s">
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="11">
+        <v>1</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G40" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="11">
-        <v>1</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="D39" s="22" t="s">
+      <c r="H40" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="E39" s="22" t="s">
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="E41" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F41" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G41" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="11">
-        <v>1</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="E40" s="22" t="s">
+      <c r="H41" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="B41" s="11">
-        <v>1</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="F41" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="17">
         <v>1</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>193</v>
+        <v>187</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>195</v>
+        <v>189</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="20">
+        <v>43</v>
+      </c>
+      <c r="B43" s="17">
         <v>1</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>198</v>
+        <v>192</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>61</v>
+        <v>194</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
+      <c r="A44" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B44" s="26"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="9"/>
-      <c r="B45" s="20">
-        <v>4</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="19"/>
+      <c r="B45" s="17">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>223</v>
+      </c>
       <c r="E45" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="F45" s="26"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
+        <v>224</v>
+      </c>
+      <c r="F45" s="23"/>
+      <c r="G45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="9"/>
-      <c r="B46" s="20">
-        <v>8</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="19"/>
+      <c r="B46" s="17">
+        <v>1</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>227</v>
+      </c>
       <c r="E46" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F46" s="26"/>
+        <v>228</v>
+      </c>
+      <c r="F46" s="23"/>
       <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
+      <c r="H46" s="10" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="9"/>
-      <c r="B47" s="20">
-        <v>4</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="F47" s="26"/>
+      <c r="B47" s="17">
+        <v>1</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F47" s="23"/>
       <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="H47" s="10" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="9"/>
-      <c r="B48" s="20">
-        <v>1</v>
+      <c r="B48" s="17">
+        <v>4</v>
       </c>
       <c r="C48" s="9"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="16"/>
       <c r="E48" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="F48" s="26"/>
+        <v>211</v>
+      </c>
+      <c r="F48" s="23"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="9"/>
-      <c r="B49" s="20">
+      <c r="B49" s="17">
         <v>1</v>
       </c>
       <c r="C49" s="9"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" s="23"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="9"/>
-      <c r="B50" s="20">
-        <v>3</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F50" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10" t="s">
-        <v>206</v>
-      </c>
+      <c r="B50" s="17">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="9"/>
-      <c r="B51" s="20">
-        <v>2</v>
+      <c r="B51" s="17">
+        <v>3</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="F51" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F51" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G51" s="10"/>
       <c r="H51" s="10" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="25"/>
-      <c r="B52" s="20">
+      <c r="A52" s="9"/>
+      <c r="B52" s="17">
         <v>2</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="9">
-        <v>50579703</v>
+      <c r="D52" s="16" t="s">
+        <v>200</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>28</v>
+        <v>201</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="G52" s="10"/>
-      <c r="H52" s="11" t="s">
-        <v>84</v>
+      <c r="H52" s="10" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="9"/>
-      <c r="B53" s="20">
-        <v>1</v>
+      <c r="A53" s="22"/>
+      <c r="B53" s="17">
+        <v>2</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="19" t="s">
-        <v>210</v>
+      <c r="D53" s="9">
+        <v>50579703</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="F53" s="26" t="s">
-        <v>114</v>
+        <v>78</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="11" t="s">
-        <v>212</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="9"/>
-      <c r="B54" s="20">
+      <c r="B54" s="17">
         <v>1</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="19" t="s">
-        <v>213</v>
+      <c r="D54" s="16" t="s">
+        <v>203</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="F54" s="26" t="s">
-        <v>118</v>
+        <v>204</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>109</v>
       </c>
       <c r="G54" s="10"/>
       <c r="H54" s="11" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="9"/>
-      <c r="B55" s="20">
-        <v>16</v>
+      <c r="B55" s="17">
+        <v>1</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="9">
-        <v>16020086</v>
+      <c r="D55" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F55" s="26"/>
+        <v>207</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>113</v>
+      </c>
       <c r="G55" s="10"/>
       <c r="H55" s="11" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="9"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="26"/>
+      <c r="B56" s="17">
+        <v>16</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="9">
+        <v>16020086</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" s="23"/>
       <c r="G56" s="10"/>
-      <c r="H56" s="11"/>
+      <c r="H56" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F57" s="26" t="s">
-        <v>125</v>
-      </c>
+      <c r="A57" s="9"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="23"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="11" t="s">
-        <v>223</v>
-      </c>
+      <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="9"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="26"/>
+      <c r="A58" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="17"/>
+      <c r="C58" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>120</v>
+      </c>
       <c r="G58" s="10"/>
-      <c r="H58" s="11"/>
+      <c r="H58" s="11" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="9"/>
-      <c r="B59" s="20"/>
+      <c r="B59" s="17"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
-      <c r="F59" s="26"/>
+      <c r="F59" s="23"/>
       <c r="G59" s="10"/>
       <c r="H59" s="11"/>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
+    <row r="60" spans="1:8">
+      <c r="A60" s="9"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="11"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:8" s="2" customFormat="1">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-    </row>
-    <row r="73" spans="7:7">
-      <c r="G73" s="3" t="s">
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:8" s="2" customFormat="1">
+      <c r="A64" s="32"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+    </row>
+    <row r="74" spans="7:7">
+      <c r="G74" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A64:G64"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A61:G61" r:id="rId1" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A62:G62" r:id="rId1" display="Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>

<commit_message>
changes CAN ports to 3 pin, Thermocouple ports to 2 pin
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/silviu/git/telemetry-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FC2164-D689-1C42-9116-B28293616D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BE6E4F-37DB-3F46-A693-F75A331B9C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="-9100" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1380,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1411,8 +1411,6 @@
     </row>
     <row r="4" spans="1:8">
       <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -1606,20 +1604,20 @@
       <c r="C13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="12">
-        <v>705510001</v>
+      <c r="D13" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>59</v>
+      <c r="H13" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1684,20 +1682,20 @@
       <c r="C16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>34</v>
+      <c r="D16" s="12">
+        <v>705510001</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>60</v>
+      <c r="H16" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2629,7 +2627,7 @@
     <row r="56" spans="1:8">
       <c r="A56" s="9"/>
       <c r="B56" s="17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>9</v>

</xml_diff>